<commit_message>
bab 5 sisa penjelasan
</commit_message>
<xml_diff>
--- a/implementasi/implementasi coding.xlsx
+++ b/implementasi/implementasi coding.xlsx
@@ -9,14 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6600" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="prepro" sheetId="1" r:id="rId1"/>
-    <sheet name="tw" sheetId="2" r:id="rId2"/>
-    <sheet name="bm25" sheetId="3" r:id="rId3"/>
-    <sheet name="pagerank" sheetId="4" r:id="rId4"/>
-    <sheet name="graf" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
+    <sheet name="class sentence" sheetId="7" r:id="rId2"/>
+    <sheet name="prepro" sheetId="1" r:id="rId3"/>
+    <sheet name="tw" sheetId="2" r:id="rId4"/>
+    <sheet name="bm25" sheetId="3" r:id="rId5"/>
+    <sheet name="pagerank" sheetId="4" r:id="rId6"/>
+    <sheet name="graf" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="160">
   <si>
     <t>def get_clean_corpus(corpus, stopwords):</t>
   </si>
@@ -246,9 +248,6 @@
     <t xml:space="preserve">class Graph:    </t>
   </si>
   <si>
-    <t xml:space="preserve">    def __init__(self, result_doc, raw_frequency, idf):</t>
-  </si>
-  <si>
     <t xml:space="preserve">        self.raw_frequency = raw_frequency</t>
   </si>
   <si>
@@ -327,9 +326,6 @@
     <t xml:space="preserve">        #calculate pagerank</t>
   </si>
   <si>
-    <t xml:space="preserve">        for i in range(100):</t>
-  </si>
-  <si>
     <t xml:space="preserve">            for item in self.doc:</t>
   </si>
   <si>
@@ -354,9 +350,6 @@
     <t xml:space="preserve">        top_pagerank = []</t>
   </si>
   <si>
-    <t xml:space="preserve">        for item in range(math.ceil(self.total_doc*0.30)):</t>
-  </si>
-  <si>
     <t xml:space="preserve">            top_pagerank.append(sorted_doc[item])</t>
   </si>
   <si>
@@ -369,9 +362,6 @@
     <t xml:space="preserve">        self.summarize = temp_summarize</t>
   </si>
   <si>
-    <t xml:space="preserve">        print(self.summarize)</t>
-  </si>
-  <si>
     <t xml:space="preserve">   </t>
   </si>
   <si>
@@ -424,6 +414,102 @@
   </si>
   <si>
     <t>#this function does cleaning, tokenize, remove stopwords, and stemming</t>
+  </si>
+  <si>
+    <t>input_document = open("bbc contoh beneran.txt", "r")</t>
+  </si>
+  <si>
+    <t>document= input_document.readline()</t>
+  </si>
+  <si>
+    <t>stopword = open("stopword_list_tala.txt", "r")</t>
+  </si>
+  <si>
+    <t>stopwords = stopword.read().split("\n")</t>
+  </si>
+  <si>
+    <t>cleaning_result = get_clean_corpus(corpus=document, stopwords=stopwords)</t>
+  </si>
+  <si>
+    <t>class Sentence:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    np.random.seed(0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    def __init__(self, id, full_sentence, clean_sentence, tokens):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        self.list_bm25 = {}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        self.pagerank_score = random.random()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        self.id = id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        self.full_sentence = full_sentence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        self.clean_sentence = clean_sentence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        self.tokens = tokens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        self.sentence_len = len(clean_sentence.split())</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        self.pagerank_score_new = 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    def calculate_bm25(self, raw_frequency, idf, doc, slen_ave):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    def calculate_new_pagerank(self, doc):</t>
+  </si>
+  <si>
+    <t>terms_frequency, df_idf  = get_term_weighting_score(cleaning_result=cleaning_result)</t>
+  </si>
+  <si>
+    <t>cr = [0.05, 0.10, 0.20, 0.30]</t>
+  </si>
+  <si>
+    <t>for crr in cr:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    print("cr : ", crr)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    percobaan = Graph(result_doc=cleaning_result, raw_frequency=terms_frequency, idf=df_idf, cr=crr)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for ringkasan in percobaan.summarize:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        print(ringkasan)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    def __init__(self, result_doc, raw_frequency, idf, cr):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        self.compression_rate = cr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        #making object sentence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        list_pgrk = [0.400827866,0.863170087,0.389187762,0.924094751,0.157640608,0.714980958,0.216858534,0.237221536,0.076112858,0.841401681]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        for i in range(4):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        for item in range(math.ceil(self.total_doc*self.compression_rate)):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        self.summarize = sorted_sum</t>
   </si>
 </sst>
 </file>
@@ -753,10 +839,421 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.85546875" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="A1:B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.140625" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>17</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>21</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>23</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>24</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>25</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>26</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>28</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>29</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>30</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>31</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>32</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,7 +1267,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -778,7 +1275,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -786,7 +1283,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -794,7 +1291,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -807,7 +1304,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="24" x14ac:dyDescent="0.25">
@@ -815,7 +1312,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -828,7 +1325,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -836,7 +1333,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -844,7 +1341,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -857,7 +1354,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -881,7 +1378,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -953,7 +1450,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="36" x14ac:dyDescent="0.25">
@@ -977,7 +1474,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="36" x14ac:dyDescent="0.25">
@@ -1001,7 +1498,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="24" x14ac:dyDescent="0.25">
@@ -1057,7 +1554,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1089,7 +1586,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1178,12 +1675,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B17" sqref="A1:B35"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,7 +1694,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1477,7 +1974,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -1576,7 +2073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1667,12 +2164,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:XFD59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1681,425 +2178,289 @@
     <col min="2" max="2" width="54.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
-        <v>1</v>
-      </c>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>2</v>
-      </c>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2" t="s">
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>13</v>
-      </c>
-      <c r="B13" s="2" t="s">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>14</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>15</v>
-      </c>
-      <c r="B15" s="2" t="s">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2" t="s">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>18</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>19</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>20</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>21</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>22</v>
-      </c>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>23</v>
-      </c>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>24</v>
-      </c>
-      <c r="B24" s="2" t="s">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>25</v>
-      </c>
-      <c r="B25" s="2" t="s">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>26</v>
-      </c>
-      <c r="B26" s="2" t="s">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>27</v>
-      </c>
-      <c r="B27" s="2" t="s">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>28</v>
-      </c>
-      <c r="B28" s="2" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>29</v>
-      </c>
-      <c r="B29" s="2" t="s">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>30</v>
-      </c>
-      <c r="B30" s="2" t="s">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>31</v>
-      </c>
-      <c r="B31" s="2" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>32</v>
-      </c>
-      <c r="B32" s="2" t="s">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>33</v>
-      </c>
-      <c r="B33" s="2" t="s">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>34</v>
-      </c>
-      <c r="B34" s="2" t="s">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>35</v>
-      </c>
-      <c r="B35" s="2" t="s">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>36</v>
-      </c>
-      <c r="B36" s="2" t="s">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>37</v>
-      </c>
-      <c r="B37" s="2" t="s">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
-        <v>38</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>39</v>
-      </c>
-      <c r="B39" s="2" t="s">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
-        <v>40</v>
-      </c>
-      <c r="B40" s="2" t="s">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
-        <v>41</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
-        <v>42</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
-        <v>43</v>
-      </c>
-      <c r="B43" s="2" t="s">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
-        <v>44</v>
-      </c>
-      <c r="B44" s="2" t="s">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
-        <v>45</v>
-      </c>
-      <c r="B45" s="2" t="s">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
-        <v>46</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
-        <v>47</v>
-      </c>
-      <c r="B47" s="2" t="s">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" s="2" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <v>48</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
-        <v>49</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
-        <v>50</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
-        <v>51</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
-        <v>52</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>